<commit_message>
removed non stare files
</commit_message>
<xml_diff>
--- a/configs/config_awaken_stand.xlsx
+++ b/configs/config_awaken_stand.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/sletizia_nrel_gov/Documents/Desktop/Main/ENDURA/awaken_lidar_processing/configs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/sletizia_nrel_gov/Documents/Desktop/Main/ENDURA/awaken_dual_doppler/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{F0C32D84-8D81-48B7-A262-049356060D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B66714-A8FB-4E74-BF29-6BDF32B02EF7}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{F0C32D84-8D81-48B7-A262-049356060D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF54250E-C4CF-4145-A752-7A87500A9AA2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -737,11 +737,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AA39"/>
+  <dimension ref="A1:Z39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N7" sqref="N7"/>
+      <selection pane="topRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,13 +756,11 @@
     <col min="10" max="10" width="51.44140625" style="5" customWidth="1"/>
     <col min="11" max="12" width="48.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="53" style="5" customWidth="1"/>
-    <col min="14" max="14" width="57.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="53" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="47.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="5"/>
+    <col min="14" max="15" width="57.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -805,9 +803,11 @@
       <c r="N1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -850,10 +850,11 @@
       <c r="N2" s="30">
         <v>20230726</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="30">
+        <v>20231023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -891,15 +892,16 @@
         <v>20260101</v>
       </c>
       <c r="M3" s="30">
-        <v>20240101</v>
+        <v>20231110</v>
       </c>
       <c r="N3" s="30">
-        <v>20240101</v>
-      </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>20231010</v>
+      </c>
+      <c r="O3" s="30">
+        <v>20231110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -942,10 +944,11 @@
       <c r="N4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -990,10 +993,11 @@
         <f>309.98-218.03</f>
         <v>91.950000000000017</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:16" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="14">
+        <v>-20.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -1036,10 +1040,11 @@
       <c r="N6" s="10">
         <v>-0.1</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="1:16" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O6" s="10">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1082,10 +1087,11 @@
       <c r="N7" s="10">
         <v>0.1</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-    </row>
-    <row r="8" spans="1:16" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
@@ -1128,10 +1134,11 @@
       <c r="N8" s="10">
         <v>-0.1</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O8" s="10">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1174,10 +1181,11 @@
       <c r="N9" s="10">
         <v>0.1</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:16" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O9" s="10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
@@ -1220,10 +1228,11 @@
       <c r="N10" s="14">
         <v>0.15</v>
       </c>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-    </row>
-    <row r="11" spans="1:16" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O10" s="14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
@@ -1266,10 +1275,11 @@
       <c r="N11" s="14">
         <v>0.1</v>
       </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-    </row>
-    <row r="12" spans="1:16" s="20" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O11" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="20" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>11</v>
       </c>
@@ -1312,10 +1322,11 @@
       <c r="N12" s="18">
         <v>0.5</v>
       </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-    </row>
-    <row r="13" spans="1:16" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O12" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>12</v>
       </c>
@@ -1358,10 +1369,11 @@
       <c r="N13" s="22">
         <v>200</v>
       </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-    </row>
-    <row r="14" spans="1:16" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>13</v>
       </c>
@@ -1404,10 +1416,11 @@
       <c r="N14" s="22">
         <v>200</v>
       </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-    </row>
-    <row r="15" spans="1:16" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O14" s="22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>14</v>
       </c>
@@ -1450,10 +1463,11 @@
       <c r="N15" s="22">
         <v>50</v>
       </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-    </row>
-    <row r="16" spans="1:16" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O15" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="24" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>15</v>
       </c>
@@ -1496,10 +1510,11 @@
       <c r="N16" s="22">
         <v>600</v>
       </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-    </row>
-    <row r="17" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="22">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1542,10 +1557,11 @@
       <c r="N17" s="7">
         <v>96</v>
       </c>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O17" s="7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1588,10 +1604,11 @@
       <c r="N18" s="7">
         <v>5000</v>
       </c>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-    </row>
-    <row r="19" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O18" s="7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1634,10 +1651,11 @@
       <c r="N19" s="7">
         <v>-25</v>
       </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-    </row>
-    <row r="20" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O19" s="7">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1680,10 +1698,11 @@
       <c r="N20" s="7">
         <v>50</v>
       </c>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-    </row>
-    <row r="21" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O20" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1726,9 +1745,11 @@
       <c r="N21" s="18">
         <v>0.1</v>
       </c>
-      <c r="O21" s="18"/>
+      <c r="O21" s="18">
+        <v>0.1</v>
+      </c>
       <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
+      <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
@@ -1738,9 +1759,8 @@
       <c r="X21" s="7"/>
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-    </row>
-    <row r="22" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1783,10 +1803,11 @@
       <c r="N22" s="7">
         <v>30</v>
       </c>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-    </row>
-    <row r="23" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O22" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1829,10 +1850,11 @@
       <c r="N23" s="7">
         <v>20</v>
       </c>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-    </row>
-    <row r="24" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O23" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1875,10 +1897,11 @@
       <c r="N24" s="7">
         <v>1</v>
       </c>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-    </row>
-    <row r="25" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1921,10 +1944,11 @@
       <c r="N25" s="7">
         <v>1</v>
       </c>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-    </row>
-    <row r="26" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1967,10 +1991,11 @@
       <c r="N26" s="7">
         <v>30</v>
       </c>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-    </row>
-    <row r="27" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O26" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -2013,10 +2038,11 @@
       <c r="N27" s="14">
         <v>0.5</v>
       </c>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-    </row>
-    <row r="28" spans="1:27" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O27" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>25</v>
       </c>
@@ -2059,10 +2085,11 @@
       <c r="N28" s="22">
         <v>25</v>
       </c>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-    </row>
-    <row r="29" spans="1:27" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O28" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>26</v>
       </c>
@@ -2105,10 +2132,11 @@
       <c r="N29" s="22">
         <v>1</v>
       </c>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-    </row>
-    <row r="30" spans="1:27" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O29" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>27</v>
       </c>
@@ -2151,10 +2179,11 @@
       <c r="N30" s="22">
         <v>99</v>
       </c>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-    </row>
-    <row r="31" spans="1:27" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O30" s="22">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
         <v>28</v>
       </c>
@@ -2197,10 +2226,11 @@
       <c r="N31" s="26">
         <v>1E-4</v>
       </c>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-    </row>
-    <row r="32" spans="1:27" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O31" s="26">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" s="28" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>29</v>
       </c>
@@ -2243,10 +2273,11 @@
       <c r="N32" s="26">
         <v>0.1</v>
       </c>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-    </row>
-    <row r="33" spans="1:16" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O32" s="26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
@@ -2289,10 +2320,11 @@
       <c r="N33" s="10">
         <v>0.25</v>
       </c>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-    </row>
-    <row r="34" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O33" s="10">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2335,10 +2367,11 @@
       <c r="N34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O34" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2381,10 +2414,11 @@
       <c r="N35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O35" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -2427,10 +2461,11 @@
       <c r="N36" s="7">
         <v>-3</v>
       </c>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O36" s="7">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>65</v>
       </c>
@@ -2473,8 +2508,11 @@
       <c r="N37" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O37" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
@@ -2489,7 +2527,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>66</v>
       </c>

</xml_diff>